<commit_message>
Bulk Import Users - Still Buggy ASF
</commit_message>
<xml_diff>
--- a/public/uploads/templates/users.xlsx
+++ b/public/uploads/templates/users.xlsx
@@ -56,16 +56,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -87,12 +87,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,19 +144,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,71 +177,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="A3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="22.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="38.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="24.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="16.89"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>35989</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>7234567890</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>